<commit_message>
upgraded to version 1.11.2.0
</commit_message>
<xml_diff>
--- a/data/xlsx/vars.xlsx
+++ b/data/xlsx/vars.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jww/Developer/python/terraformer/data/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jww/Developer/python/tabular-terraform/data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{318114A4-14E1-794D-A167-7A030ABC99AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FD44F2B-DF6A-904B-8396-EDFCAA8BCCA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14780" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -458,9 +458,6 @@
     <t>ibm_is_instance.webappserver-zone1[0].primary_network_interface[0].primary_ipv4_address</t>
   </si>
   <si>
-    <t>ansible-playbook</t>
-  </si>
-  <si>
     <t>zone1-bastionserver</t>
   </si>
   <si>
@@ -483,6 +480,9 @@
   </si>
   <si>
     <t>app_name</t>
+  </si>
+  <si>
+    <t>ansible</t>
   </si>
 </sst>
 </file>
@@ -983,7 +983,7 @@
         <v>27</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>108</v>
@@ -997,7 +997,7 @@
         <v>28</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>109</v>
@@ -1710,7 +1710,7 @@
         <v>80</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>105</v>
@@ -1728,7 +1728,7 @@
         <v>80</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>96</v>
@@ -1764,7 +1764,7 @@
         <v>80</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>97</v>
@@ -1806,7 +1806,7 @@
         <v>80</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>91</v>
@@ -1842,7 +1842,7 @@
         <v>80</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>98</v>
@@ -1914,10 +1914,10 @@
         <v>80</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D21" s="1"/>
     </row>

</xml_diff>